<commit_message>
[AS]- Done Refactoring in MCA, UserDetailsPS, SearchOnlineAccount_2 and LifeSpanFlow
</commit_message>
<xml_diff>
--- a/TestDocuments/OrangeDecomm_ Test_Cases/MCA_Test_cases_V0.1.xlsx
+++ b/TestDocuments/OrangeDecomm_ Test_Cases/MCA_Test_cases_V0.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="133">
   <si>
     <t>Test Cases - MCA.CreateUpdateMsisdnProfile</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>User should be able to disconnect Inactive MSISDN from the First and Second Portal ID.</t>
+  </si>
+  <si>
+    <t>Install - POST-PAY</t>
   </si>
 </sst>
 </file>
@@ -894,28 +897,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF99"/>
@@ -999,11 +980,33 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1401,46 +1404,46 @@
     <mergeCell ref="G7:J7"/>
   </mergeCells>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I12">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H12">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1450,11 +1453,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3725,14 +3728,193 @@
       <c r="H127" s="8"/>
       <c r="I127" s="4"/>
     </row>
+    <row r="128" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B128" s="25"/>
+      <c r="C128" s="25"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="25"/>
+      <c r="H128" s="25"/>
+      <c r="I128" s="26"/>
+    </row>
+    <row r="129" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>112</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8"/>
+      <c r="F129" s="8"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>113</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D130" s="8"/>
+      <c r="E130" s="8"/>
+      <c r="F130" s="8"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>114</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D131" s="8"/>
+      <c r="E131" s="8"/>
+      <c r="F131" s="8"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="8"/>
+      <c r="I131" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <v>115</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <v>116</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D133" s="8"/>
+      <c r="E133" s="8"/>
+      <c r="F133" s="8"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
+        <v>117</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C134" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+      <c r="F134" s="8"/>
+      <c r="G134" s="8"/>
+      <c r="H134" s="8"/>
+      <c r="I134" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <v>118</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8"/>
+      <c r="F135" s="8"/>
+      <c r="G135" s="8"/>
+      <c r="H135" s="8"/>
+      <c r="I135" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <v>119</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D136" s="8"/>
+      <c r="E136" s="8"/>
+      <c r="F136" s="8"/>
+      <c r="G136" s="8"/>
+      <c r="H136" s="8"/>
+      <c r="I136" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <v>120</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+      <c r="F137" s="8"/>
+      <c r="G137" s="8"/>
+      <c r="H137" s="8"/>
+      <c r="I137" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A44:I44"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A34:I34"/>
+  <mergeCells count="15">
+    <mergeCell ref="A128:I128"/>
     <mergeCell ref="A106:I106"/>
     <mergeCell ref="A116:I116"/>
     <mergeCell ref="A54:I54"/>
@@ -3741,6 +3923,12 @@
     <mergeCell ref="A76:I76"/>
     <mergeCell ref="A86:I86"/>
     <mergeCell ref="A96:I96"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A34:I34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>